<commit_message>
IMU V2 Artwork Update
-Added Board radius of .25in
- converted to 2 layer board
</commit_message>
<xml_diff>
--- a/Photon_Dev/IMU_External/IMU_External_BOM.xlsx
+++ b/Photon_Dev/IMU_External/IMU_External_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
   <si>
     <t>Item</t>
   </si>
@@ -293,12 +293,6 @@
     <t>LSM9DS1</t>
   </si>
   <si>
-    <t>IMU External PCB V1.0</t>
-  </si>
-  <si>
-    <t>Wednesday 3/1/16</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -350,10 +344,13 @@
     <t>R3, R4</t>
   </si>
   <si>
-    <t>**Leave R1 and R2 unpopulated.</t>
-  </si>
-  <si>
     <t>* Suitable generic replacements/substitutions are acceptable for all components except Item #7.</t>
+  </si>
+  <si>
+    <t>IMU External PCB V2.0</t>
+  </si>
+  <si>
+    <t>Sunday 4/10/16</t>
   </si>
 </sst>
 </file>
@@ -1589,7 +1586,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1607,7 +1604,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1615,7 +1612,7 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1658,13 +1655,13 @@
         <v>84</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G11" s="23" t="s">
         <v>50</v>
@@ -1684,10 +1681,10 @@
         <v>3</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F12" s="27">
         <v>61900411021</v>
@@ -1703,22 +1700,22 @@
         <v>1</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G13" s="25">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="H13" s="26">
-        <f>G13*B13</f>
+        <f t="shared" ref="H13:H18" si="0">G13*B13</f>
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
@@ -1733,19 +1730,19 @@
         <v>8</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G14" s="25">
         <v>0.02</v>
       </c>
       <c r="H14" s="26">
-        <f>G14*B14</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
@@ -1757,22 +1754,22 @@
         <v>5</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G15" s="25">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="H15" s="26">
-        <f>G15*B15</f>
+        <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
     </row>
@@ -1784,22 +1781,22 @@
         <v>2</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G16" s="25">
         <v>1.2E-2</v>
       </c>
       <c r="H16" s="26">
-        <f>G16*B16</f>
+        <f t="shared" si="0"/>
         <v>2.4E-2</v>
       </c>
     </row>
@@ -1811,22 +1808,22 @@
         <v>2</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G17" s="25">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H17" s="26">
-        <f>G17*B17</f>
+        <f t="shared" si="0"/>
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
@@ -1841,10 +1838,10 @@
         <v>36</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F18" s="22" t="s">
         <v>89</v>
@@ -1853,18 +1850,13 @@
         <v>5.74</v>
       </c>
       <c r="H18" s="34">
-        <f>G18*B18</f>
+        <f t="shared" si="0"/>
         <v>5.74</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:8">

</xml_diff>